<commit_message>
further tweaks to art catalogues
</commit_message>
<xml_diff>
--- a/excel_files/AuctionCatalogues.sothebysParkeBernet.xlsx
+++ b/excel_files/AuctionCatalogues.sothebysParkeBernet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="525">
   <si>
     <t>Sublibrary</t>
   </si>
@@ -94,792 +94,804 @@
     <t>ARTBL</t>
   </si>
   <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Chinese snuff bottles, jade carvings, archaic bronzes, sculpture, ceramics, works of art and paintings</t>
+  </si>
+  <si>
+    <t>nyu</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Sotheby Parke Bernet Inc</t>
+  </si>
+  <si>
+    <t>[1977?]</t>
+  </si>
+  <si>
+    <t>© 1977</t>
+  </si>
+  <si>
+    <t>approximately 156 pages</t>
+  </si>
+  <si>
+    <t>24 cm</t>
+  </si>
+  <si>
+    <t>including fine snuff bottles from the collection of the late E. Lucille Parker, Erie, Pennsylvania (part II); Chinese paintings by Wên Chêng-ming, Tao Chi, Wang Yuan-ch'i, Wang Hui, Ch'i Pai-shih, Chang Ta-ch'ien, Hsü Pei-hung and other artists; jade carvings: a fine white jade rustic brush washer, 18th century; archaic bronzes: an important bronze fang yi, Shang dynasty; a well-cast bronze wine vessel (tsun), Shang dynasty; a rare bronze chariot shaft fitting, Western Chou dynasty; T'ang gilt bronze : a rare gilt bronze stemcup, T'ang dynasty;  sculpture:  a large black marble lion, T'ang dynasty; a large stone figure of a lady, T'ang dynasty; a large stone figure of a mourner, T'ang dynasty; early pottery figures: a large painted gray pottery equestrian, Wei dynasty; a printed gray pottery horse, Han dynasty;  Liao pottery: a fine pair of green glazed pottery flasks, Liao dynasty; various Sung and later pottery and porcelain; property from the estates of Mr. Robert Dinolt, Putnam, Connecticut; Greta S. Heckett, Pittsburgh, Pa.; Frank V. Gill, New York, New York; John H. Wilkins, Chevy Chase, Md.; Martha E. Dick, Reading, Pa. and other owners</t>
+  </si>
+  <si>
+    <t>19770601, 19770602</t>
+  </si>
+  <si>
+    <t>water damage throughout; some pages stuck together</t>
+  </si>
+  <si>
+    <t>Donated by the Ashmolean Museum.</t>
+  </si>
+  <si>
+    <t>Oriental rugs and carpets</t>
+  </si>
+  <si>
+    <t>property of various owners</t>
+  </si>
+  <si>
+    <t>approximately 88 pages</t>
+  </si>
+  <si>
+    <t>19770603</t>
+  </si>
+  <si>
+    <t>Korean works of art</t>
+  </si>
+  <si>
+    <t>approximately 68 pages</t>
+  </si>
+  <si>
+    <t>including important Lo-Lang lacquer cup, old Silla period gold jewelry, highly important Silla silver belt, Silla gilt bronzes, good Koryŏ celadons, including Kangjin kilns pieces, Koryŏ bronzes; rare Yi silver cup and pick, fine Yi red wares, Yi blue and white wares</t>
+  </si>
+  <si>
+    <t>19770614</t>
+  </si>
+  <si>
+    <t>Japanese and other Asian works of art</t>
+  </si>
+  <si>
+    <t>approximately 144 pages</t>
+  </si>
+  <si>
+    <t>Korean, Indian, Kashmire, tibetan, Nepalese, Southeast Asian works of art; Japanese prints, drawings, paintings, screens, illustrated books, reference books, swords, fittings, armour, ceramics and porcelains, ivories, metalwork, sculpture, wood and ivory netsuke, inro, lacquer especially good Indian and Southeast Asian stone sculpture, highly important Kashmir figure of Raktalokesvara, good 18th century Tibetan tanka of a Mahāsiddha, a fine pair of screens attribted to Kano Tanyu, highly important Nara dry lacquer figure of Monju</t>
+  </si>
+  <si>
+    <t>19770614, 19770615</t>
+  </si>
+  <si>
+    <t>approximately 72 pages</t>
+  </si>
+  <si>
+    <t>19771001</t>
+  </si>
+  <si>
+    <t>Japanese and other Asian works of art and a highly important American collection of early Japanese Buddhist &amp; Shinto paintings and sculptures (Part 1)</t>
+  </si>
+  <si>
+    <t>approximately 212 pages</t>
+  </si>
+  <si>
+    <t>a monumental Heian wood figure of a bodhisattva; a series of Chola and other Indian bronzes and stone; an early  Nepalese bronze of Syamatara; a fine Javanese bronze of Prajñāpāramitā; Japanese printings, sculpture, bronzes, lacquer, swords, fittings, prints, drawings, screens, ceramics, netsuke, inro, lacquer; Korean, Tibetan, Nepaliese, Indian and Southeast Asian works of art</t>
+  </si>
+  <si>
+    <t>19771103, 19771104</t>
+  </si>
+  <si>
+    <t>The contents of Mountain Crest, the collection of Mrs. Loyce Mayfield</t>
+  </si>
+  <si>
+    <t>approximately 96 pages</t>
+  </si>
+  <si>
+    <t>a fine collection of birds modelled by Dorothy Doughty and Edward Marshall Boehm, oriental works of arts, fine oriental rugs and carpets, Paul Storr George III silver soup tureen and cover, furniture and other decorative arts</t>
+  </si>
+  <si>
+    <t>19770610, 10770611</t>
+  </si>
+  <si>
+    <t>Chinese ceramics and works of art</t>
+  </si>
+  <si>
+    <t>approximately 116 pages</t>
+  </si>
+  <si>
+    <t>19771105</t>
+  </si>
+  <si>
+    <t>Chinese snuff bottles, jades, paintings, textiles and other works of art</t>
+  </si>
+  <si>
+    <t>[1978?]</t>
+  </si>
+  <si>
+    <t>© 1978</t>
+  </si>
+  <si>
+    <t>approximately 106 pages</t>
+  </si>
+  <si>
+    <t>19780125, 19780126</t>
+  </si>
+  <si>
+    <t>approximately 32 pages</t>
+  </si>
+  <si>
+    <t>19780304</t>
+  </si>
+  <si>
+    <t>19780128</t>
+  </si>
+  <si>
+    <t>Fine oriental miniatures, manuscripts, Islamic works of art, and 19th century paintings</t>
+  </si>
+  <si>
+    <t>[1979?]</t>
+  </si>
+  <si>
+    <t>© 1979</t>
+  </si>
+  <si>
+    <t>approximately 126 pages</t>
+  </si>
+  <si>
+    <t>19791214</t>
+  </si>
+  <si>
+    <t>Fine oriental miniatures, manuscripts, Islamic works of art, including the Fraser album</t>
+  </si>
+  <si>
+    <t>[1980?]</t>
+  </si>
+  <si>
+    <t>© 1980</t>
+  </si>
+  <si>
+    <t>approximately 136 pages</t>
+  </si>
+  <si>
+    <t>[property of various owners] including: property of Mr. Malcolm Fraser, property from the Estate of Nelson A. Rockefeller, property from the Estate of Mrs Benjamin Sonnenberg, property from the Hagop Kevorkian Fund</t>
+  </si>
+  <si>
+    <t>4493Y</t>
+  </si>
+  <si>
+    <t>19801209</t>
+  </si>
+  <si>
+    <t>Fine oriental miniatures, manuscripts, Islamic works of art</t>
+  </si>
+  <si>
+    <t>[1981?]</t>
+  </si>
+  <si>
+    <t>© 1981</t>
+  </si>
+  <si>
+    <t>approximately 120 pages</t>
+  </si>
+  <si>
+    <t>[property of various owners] including: the property of Mrs. Henry R. Gutnayer, New York; the property of Mr. and Mrs. Eugene Bernat; the property of Mr. Jack Josephson; the property of a New York collector; the property from the estate of Evelyn C. Byng</t>
+  </si>
+  <si>
+    <t>4618Y</t>
+  </si>
+  <si>
+    <t>19810521</t>
+  </si>
+  <si>
+    <t>[property of various owners] including: the property of Mr. T.B. Kahle, the property from the estate of Laila Y. Mathers, the property of Dr. and Mrs. Warren Baker, the property from the collection of the late Mr. Carleton Richmond</t>
+  </si>
+  <si>
+    <t>4756Y</t>
+  </si>
+  <si>
+    <t>19811210</t>
+  </si>
+  <si>
+    <t>Fine oriental miniatures, manuscripts and Islamic works of art</t>
+  </si>
+  <si>
+    <t>[1982?]</t>
+  </si>
+  <si>
+    <t>© 1982</t>
+  </si>
+  <si>
+    <t>approximately 104 pages</t>
+  </si>
+  <si>
+    <t>4867Y</t>
+  </si>
+  <si>
+    <t>19820519</t>
+  </si>
+  <si>
+    <t>Chinese and Japanese paintings, works of art and furniture</t>
+  </si>
+  <si>
+    <t>[1983?]</t>
+  </si>
+  <si>
+    <t>© 1983</t>
+  </si>
+  <si>
+    <t>approximately 100 pages</t>
+  </si>
+  <si>
+    <t>property of various owners including: property of the Newark Museum, property of the estate of Sophie H. Gimbel, property of the estate of Charlotte V. Bergen, Bernardsville, New Jersey. Sold by the order of the Trustees, Fidelity Union Bank, Newark, New Jersey. Property of Yves Saint Laurent, Inc. Property of the Albany Institute of History and Art. Property from the collection of the Late  Dr. and Mrs. Louis E. Wolferz, sold by order of the Heirs. Property of the estate of R. Foster Reynolds, Providence, Rhode Island. Property from the collection of Captain S. N. Ferris Luboshez USN (Ret'd). Property from the estate of Anne Burnett Tandy, Fort Worth, Texas.</t>
+  </si>
+  <si>
+    <t>19830226</t>
+  </si>
+  <si>
+    <t>Fine Japanese works of art including lacquer, ceramics, metalwork, enamels and paintings</t>
+  </si>
+  <si>
+    <t>[1984?]</t>
+  </si>
+  <si>
+    <t>© 1984</t>
+  </si>
+  <si>
+    <t>approximately 124 pages</t>
+  </si>
+  <si>
+    <t>19840331</t>
+  </si>
+  <si>
+    <t>Fine Oriental rugs and carpets</t>
+  </si>
+  <si>
+    <t>approximately 132 pages</t>
+  </si>
+  <si>
+    <t>property of various owners including: The Austin Family , Rosemont, Pennsylvania; The estate of Vladimir M. Eitingon; The estate of Reverend Joseph Madigan; The Ten Eyck Family, New York State; A London publishing house; A European gentleman</t>
+  </si>
+  <si>
+    <t>19840519</t>
+  </si>
+  <si>
+    <t>Fine Japanese prints, paintings, screens and decorative works of art</t>
+  </si>
+  <si>
+    <t>Including property from the Fichter collection of landscape prints and from the collection of Charles Hovey Pepper</t>
+  </si>
+  <si>
+    <t>27cm</t>
+  </si>
+  <si>
+    <t>SHAKUDO 5234</t>
+  </si>
+  <si>
+    <t>19841109, 19841110</t>
+  </si>
+  <si>
+    <t>The Salvatore J. Tarantino collection of woodblock prints by Ando Hiroshige (1797-1858) and fine woodblock prints, paintings and screens from various owners</t>
+  </si>
+  <si>
+    <t>Sotheby's Inc</t>
+  </si>
+  <si>
+    <t>[1985?]</t>
+  </si>
+  <si>
+    <t>© 1985</t>
+  </si>
+  <si>
+    <t>approximately 140 pages</t>
+  </si>
+  <si>
+    <t>TARANTINO 5385</t>
+  </si>
+  <si>
+    <t>19851106, 19851107</t>
+  </si>
+  <si>
+    <t>Fine Chinese snuff bottles</t>
+  </si>
+  <si>
+    <t>from the collection of Dr. Paula Hallett, immediately followed by snuff bottles the property of various owners</t>
+  </si>
+  <si>
+    <t>approximately 64 pages</t>
+  </si>
+  <si>
+    <t>MATRIX 5416</t>
+  </si>
+  <si>
+    <t>19851202</t>
+  </si>
+  <si>
+    <t>Fine Japanese prints, paintings, screens and works of art</t>
+  </si>
+  <si>
+    <t>[1986?]</t>
+  </si>
+  <si>
+    <t>© 1986</t>
+  </si>
+  <si>
+    <t>approximately  pages</t>
+  </si>
+  <si>
+    <t>YABU 5488</t>
+  </si>
+  <si>
+    <t>19860924</t>
+  </si>
+  <si>
+    <t>Fine Chinese paintings</t>
+  </si>
+  <si>
+    <t>Property of various owners, including the Kimbell Art Foundation, Fort Worth, Texas; Andrew Franklin, C.V.O. C.B.E., former British China  Consular Service; a European collection</t>
+  </si>
+  <si>
+    <t>[1987?]</t>
+  </si>
+  <si>
+    <t>© 1987</t>
+  </si>
+  <si>
+    <t>SONG KE 5591</t>
+  </si>
+  <si>
+    <t>19870602</t>
+  </si>
+  <si>
+    <t>Southeby's Arcade Auctions</t>
+  </si>
+  <si>
+    <t>Oriental and European rugs and carpets</t>
+  </si>
+  <si>
+    <t>approximately 44 pages</t>
+  </si>
+  <si>
+    <t>property of various owners including: property of the Metropolitan Museum of Art; property from the estate of Milford S. Worth; property of an Eastern private collector; property of a private collector, Pennsylvania</t>
+  </si>
+  <si>
+    <t>19870916</t>
+  </si>
+  <si>
+    <t>[1988?]</t>
+  </si>
+  <si>
+    <t>© 1988</t>
+  </si>
+  <si>
+    <t>approximately 36 pages</t>
+  </si>
+  <si>
+    <t>19880322</t>
+  </si>
+  <si>
+    <t>approximately 42 pages</t>
+  </si>
+  <si>
+    <t>property of various owners, including: the estate of George Kirkland Bishop; property from the estate of Caroline Ryan Foulke; property from the Estate of Sylvia Montag  Ferst; property of the Pacific Asia Museum, Pasadena, California; property from the estate of Belle Linsky, sold by the executors, Muriel Karasik and William D. Zabel; property from the Estate of Mrs. George Devendorf</t>
+  </si>
+  <si>
+    <t>19880928</t>
+  </si>
+  <si>
+    <t>Fine netsuke, inro and lacquer from the estate of Madelyn Hickmott</t>
+  </si>
+  <si>
+    <t>Sold for the benefit of the Hartford Foundation for Public Giving</t>
+  </si>
+  <si>
+    <t>[1989?]</t>
+  </si>
+  <si>
+    <t>© 1989</t>
+  </si>
+  <si>
+    <t>approximately 118 pages</t>
+  </si>
+  <si>
+    <t>HICKMOTT 5811</t>
+  </si>
+  <si>
+    <t>19890208</t>
+  </si>
+  <si>
+    <t>Fine Chinese decorative works of art</t>
+  </si>
+  <si>
+    <t>approximately 218 pages</t>
+  </si>
+  <si>
+    <t>property of various owners including: property of the Traphagen School Museum, New York; property from the estate of Madelyn Hickmott; property from the estate of William R. Lipscomb; property from a Miami Beach estate; property from a Northwest institution; property from the estate of Mr. and Mrs. Oliver Smalley; property from the collection of Philip Swingle</t>
+  </si>
+  <si>
+    <t>MEIXIAN 5897</t>
+  </si>
+  <si>
+    <t>19890928, 19890929</t>
+  </si>
+  <si>
+    <t>[1990?]</t>
+  </si>
+  <si>
+    <t>© 1990</t>
+  </si>
+  <si>
+    <t>approximately 230 pages</t>
+  </si>
+  <si>
+    <t>including: property from the estate of Frances C. Albee; property from the collection of Mrs. Elva Bernat; property from the collection of Mr. and Mrs. Jacques Brazy; property from the collection of John T. Dorrance, Jr.; property of a Florida collector; property from the collection of Maitland Lee Griggs; property from the estate of Madelyn Hickmott; property from the collection of Stanley J. Love; property from a Miami Beach estate; property from a private New Jersey collection; property from the estate of Mr. and Mrs. Oliver Smalley; property from the Smith-Walker Foundation; property from the collection of Ira H. Van Cleave; property from the collection of Frederick J. and Antoinette H. Van Syke</t>
+  </si>
+  <si>
+    <t>TINGQUA 5996</t>
+  </si>
+  <si>
+    <t>19900411, 19900412</t>
+  </si>
+  <si>
+    <t>approximately 174 pages</t>
+  </si>
+  <si>
+    <t>including property From the collection of the late Victoria Contag, formerly on loan to the Nelson-Atkins Museum. Kansas City, Missouri; Property From a European collection; property from an important private collection; property of the Sixuezhai collection</t>
+  </si>
+  <si>
+    <t>QICHANG 6027</t>
+  </si>
+  <si>
+    <t>19900530</t>
+  </si>
+  <si>
+    <t>approximately 210 pages</t>
+  </si>
+  <si>
+    <t>including property from the collection of the late Victoria Contag; property from the collection of John T. Dorrance; property from the collection of Dr. Robert J. Fanning; property from the estate of Richard B. Gump; property from a private Midwest collection; property of Mrs. Rafi Y. Mottahedeh; property of Sotheby's; property from the estate of Anoinette H. Van Slyke; property from the estate of Gordon Bailey Washburn</t>
+  </si>
+  <si>
+    <t>TAINAN 6074</t>
+  </si>
+  <si>
+    <t>19901018, 19901019</t>
+  </si>
+  <si>
+    <t>The Carter Burden collection of Indian paintings</t>
+  </si>
+  <si>
+    <t>[1991?]</t>
+  </si>
+  <si>
+    <t>© 1991</t>
+  </si>
+  <si>
+    <t>approximately 80 pages</t>
+  </si>
+  <si>
+    <t>PAHARI 6122</t>
+  </si>
+  <si>
+    <t>19910327</t>
+  </si>
+  <si>
+    <t>Indian and Southeast Asian art</t>
+  </si>
+  <si>
+    <t>including property of William H. Wolff, Inc.; property of Richard B. Gump, San Francisco; property from the collection of Carter Burden; property sold by the Los Angeles County Museum of Art to benefit future acquisitions; property of Dr. Kaywin Lehman Smith; property of the Ernest Erickson Foundation; works of art from the collection of the late Edgar J. Kaufman, Jr.</t>
+  </si>
+  <si>
+    <t>WOLFF 6146</t>
+  </si>
+  <si>
+    <t>Egyptian, Greek, Etruscan, Roman and Western Asiatic antiquities and Islamic works of art</t>
+  </si>
+  <si>
+    <t>including: a Roman bronze center table; an Attic marble grave stele, circa 360 B.C.; an Egyptian Chephren diorite jar, dynasty I-II; an Attic red-figure cup attributed to the school of Makron; a Roman marble head of Apollo; a Syrian limestone head of a god or prince; an Egyptian bronze mongoose; an Apulian red-figure pelike attibuted to the Lycurgus painter; a Cycladic marble pyxis, early bronze age II; a Roman marble cinerary vase, Flavian period; an Egyptian limestone relief of Akhenaten and Meritaten; a Roman bronze figure of Jupiter; an Egyptian limestone relief of the god Tutu; a Roman marble figure of Polyhymia</t>
+  </si>
+  <si>
+    <t>SENWOSRET 6196</t>
+  </si>
+  <si>
+    <t>19910618</t>
+  </si>
+  <si>
+    <t>[1992?]</t>
+  </si>
+  <si>
+    <t>© 1992</t>
+  </si>
+  <si>
+    <t>approximately 180 pages</t>
+  </si>
+  <si>
+    <t>XUANZAI 6306</t>
+  </si>
+  <si>
+    <t>19920601</t>
+  </si>
+  <si>
+    <t>Fine Chinese ceramics and works of art</t>
+  </si>
+  <si>
+    <t>including property from the collection of Maude Bouvier-Davis; property from the collection of Marlene Casey; property from a California estate; property from a Canadian collector; property from a Connecticut private collection; property from the collection of Sidney Day; property from an East Coast private collection; property from the estate of Helen Griiser; property of a Hong Kong private collection; property from the estate of William E. Little; property from the estate of Paul Martini, formerly in the collection of William Goadby Loew; property of a Maryland estate; property formerly in the estate of John Alex McCone, sold for the benefit of the McCone Foundation; property from the estate of Isabelle M. Murphy; property of a private New Jersey collection; property from a private collection; property from the collection of Adele Simpson; property of a southern museum; property from the estate of Thomas van Deusen; property from a Virginia private collection; property from the estate of S. Fulleron Weaver, East Hampton, New York; property from the estate of Ruth Weiss; property from the estate of William H. Wolff</t>
+  </si>
+  <si>
+    <t>QUEMOY 6308</t>
+  </si>
+  <si>
+    <t>19920603</t>
+  </si>
+  <si>
+    <t>Decorative works of art</t>
+  </si>
+  <si>
+    <t>Chinese, Japanese and Korean</t>
+  </si>
+  <si>
+    <t>approximately 190 pages</t>
+  </si>
+  <si>
+    <t>MONKEY 6312</t>
+  </si>
+  <si>
+    <t>19920606</t>
+  </si>
+  <si>
+    <t>[2001?]</t>
+  </si>
+  <si>
+    <t>152 pages</t>
+  </si>
+  <si>
+    <t>ELY 7622</t>
+  </si>
+  <si>
+    <t>20010322</t>
+  </si>
+  <si>
+    <t>236 pages</t>
+  </si>
+  <si>
+    <t>including important snuff bottles from a distinguished Asian collection</t>
+  </si>
+  <si>
+    <t>PRIMUS 7696</t>
+  </si>
+  <si>
+    <t>20010919</t>
+  </si>
+  <si>
+    <t>[2000?]</t>
+  </si>
+  <si>
+    <t>148 pages</t>
+  </si>
+  <si>
+    <t>ARUNDEL 7445</t>
+  </si>
+  <si>
+    <t>20000322</t>
+  </si>
+  <si>
+    <t>Important Chinese snuff bottles</t>
+  </si>
+  <si>
+    <t>[1997?]</t>
+  </si>
+  <si>
+    <t>© 1997</t>
+  </si>
+  <si>
+    <t>approximately 128 pages</t>
+  </si>
+  <si>
+    <t>including property from the John Franklin Dodge and Isabel Beatty Dodge Collection formed before 1965 (The Dodge Collection); property from The Pauline Lester Collection (Pauline Lester); property from a private Mid-Western American collection (The Mid-Western Collection); property from a private Canadian collection formed in Pekin before 1955 (The Canadian Collection); property from a private British Columbia Collection (The B.C. Collection); property from a private San Francisco collection (The S. F. Collection)</t>
+  </si>
+  <si>
+    <t>GOURD 6962</t>
+  </si>
+  <si>
+    <t>19970317</t>
+  </si>
+  <si>
+    <t>Fine Chinese Paintings</t>
+  </si>
+  <si>
+    <t>Asian Art</t>
+  </si>
+  <si>
+    <t>[1995?]</t>
+  </si>
+  <si>
+    <t>© 1995</t>
+  </si>
+  <si>
+    <t>approximately 160 pages</t>
+  </si>
+  <si>
+    <t>QIYUE 6738</t>
+  </si>
+  <si>
+    <t>19950918</t>
+  </si>
+  <si>
+    <t>[1993?]</t>
+  </si>
+  <si>
+    <t>© 1993</t>
+  </si>
+  <si>
+    <t>approximately 50 pages</t>
+  </si>
+  <si>
+    <t>including property of a private American collector</t>
+  </si>
+  <si>
+    <t>SHIPJANGSAENG 6441</t>
+  </si>
+  <si>
+    <t>19930618</t>
+  </si>
+  <si>
+    <t>Fine netsuke, inro and related works of art</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>MIAMI 5548</t>
+  </si>
+  <si>
+    <t>19870112</t>
+  </si>
+  <si>
+    <t>The Anne Paul Brinkman collection</t>
+  </si>
+  <si>
+    <t>ne</t>
+  </si>
+  <si>
+    <t>Amsterdam</t>
+  </si>
+  <si>
+    <t>Sotheby's Amsterdam B.V.</t>
+  </si>
+  <si>
+    <t>[2002?]</t>
+  </si>
+  <si>
+    <t>190 pages</t>
+  </si>
+  <si>
+    <t>AM0856</t>
+  </si>
+  <si>
+    <t>20020917</t>
+  </si>
+  <si>
+    <t>English / Dutch</t>
+  </si>
+  <si>
+    <t>Rugs and carpets</t>
+  </si>
+  <si>
+    <t>From the collection of the late Mr. P. Otten, Amsterdam.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tapijten </t>
+  </si>
+  <si>
+    <t>Uit de verzameling van wijlen de heer Mr. P. Otten te Amsterdam</t>
+  </si>
+  <si>
+    <t>Sotheby Mak Van Waay B.V.</t>
+  </si>
+  <si>
+    <t>12 pages</t>
+  </si>
+  <si>
+    <t>19870706</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Collection d'un amateur</t>
+  </si>
+  <si>
+    <t>Rouen 1680-1740: de la première porcelaine à l'âge d'or de la faïence</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Sotheby's France SA</t>
+  </si>
+  <si>
+    <t>[2008?]</t>
+  </si>
+  <si>
+    <t>166 pages</t>
+  </si>
+  <si>
+    <t>PF8025 ROUEN</t>
+  </si>
+  <si>
+    <t>20080618</t>
+  </si>
+  <si>
+    <t>Collection de monsieur et madame Luigi Anton Laura</t>
+  </si>
+  <si>
+    <t>Important mobilier, objets d'art et porcelaines de Chine</t>
+  </si>
+  <si>
+    <t>334 pages</t>
+  </si>
+  <si>
+    <t>28cm</t>
+  </si>
+  <si>
+    <t>PF1001 LAURA</t>
+  </si>
+  <si>
+    <t>20010627</t>
+  </si>
+  <si>
+    <t>Fine modern Chinese oil paintings, drawings and watercolours</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>Taipei</t>
+  </si>
+  <si>
+    <t>Sotheby's Taiwan Ltd.</t>
+  </si>
+  <si>
+    <t>SANXIA</t>
+  </si>
+  <si>
+    <t>19930418</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>La collezione Colasanti-Moore, Piazza dell'Orologio, Roma</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>Milan</t>
+  </si>
+  <si>
+    <t>Sotheby's Italia</t>
+  </si>
+  <si>
+    <t>181 pages</t>
+  </si>
+  <si>
+    <t>MI166 FABIOLA</t>
+  </si>
+  <si>
+    <t>20000229</t>
+  </si>
+  <si>
     <t>eng</t>
   </si>
   <si>
-    <t>Chinese snuff bottles, jade carvings, archaic bronzes, sculpture, ceramics, works of art and paintings</t>
-  </si>
-  <si>
-    <t>nyu</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>Sotheby Parke Bernet Inc</t>
-  </si>
-  <si>
-    <t>[1977?]</t>
-  </si>
-  <si>
-    <t>© 1977</t>
-  </si>
-  <si>
-    <t>approximately 156 pages</t>
-  </si>
-  <si>
-    <t>24 cm</t>
-  </si>
-  <si>
-    <t>including fine snuff bottles from the collection of the late E. Lucille Parker, Erie, Pennsylvania (part II); Chinese paintings by Wên Chêng-ming, Tao Chi, Wang Yuan-ch'i, Wang Hui, Ch'i Pai-shih, Chang Ta-ch'ien, Hsü Pei-hung and other artists; jade carvings: a fine white jade rustic brush washer, 18th century; archaic bronzes: an important bronze fang yi, Shang dynasty; a well-cast bronze wine vessel (tsun), Shang dynasty; a rare bronze chariot shaft fitting, Western Chou dynasty; T'ang gilt bronze : a rare gilt bronze stemcup, T'ang dynasty;  sculpture:  a large black marble lion, T'ang dynasty; a large stone figure of a lady, T'ang dynasty; a large stone figure of a mourner, T'ang dynasty; early pottery figures: a large painted gray pottery equestrian, Wei dynasty; a printed gray pottery horse, Han dynasty;  Liao pottery: a fine pair of green glazed pottery flasks, Liao dynasty; various Sung and later pottery and porcelain; property from the estates of Mr. Robert Dinolt, Putnam, Connecticut; Greta S. Heckett, Pittsburgh, Pa.; Frank V. Gill, New York, New York; John H. Wilkins, Chevy Chase, Md.; Martha E. Dick, Reading, Pa. and other owners</t>
-  </si>
-  <si>
-    <t>19770601, 19770602</t>
-  </si>
-  <si>
-    <t>water damage throughout; some pages stuck together</t>
-  </si>
-  <si>
-    <t>Donated by the Ashmolean Museum.</t>
-  </si>
-  <si>
-    <t>Oriental rugs and carpets</t>
-  </si>
-  <si>
-    <t>property of various owners</t>
-  </si>
-  <si>
-    <t>approximately 88 pages</t>
-  </si>
-  <si>
-    <t>19770603</t>
-  </si>
-  <si>
-    <t>Korean works of art</t>
-  </si>
-  <si>
-    <t>approximately 68 pages</t>
-  </si>
-  <si>
-    <t>including important Lo-Lang lacquer cup, old Silla period gold jewelry, highly important Silla silver belt, Silla gilt bronzes, good Koryŏ celadons, including Kangjin kilns pieces, Koryŏ bronzes; rare Yi silver cup and pick, fine Yi red wares, Yi blue and white wares</t>
-  </si>
-  <si>
-    <t>19770614</t>
-  </si>
-  <si>
-    <t>Japanese and other Asian works of art</t>
-  </si>
-  <si>
-    <t>approximately 144 pages</t>
-  </si>
-  <si>
-    <t>Korean, Indian, Kashmire, tibetan, Nepalese, Southeast Asian works of art; Japanese prints, drawings, paintings, screens, illustrated books, reference books, swords, fittings, armour, ceramics and porcelains, ivories, metalwork, sculpture, wood and ivory netsuke, inro, lacquer especially good Indian and Southeast Asian stone sculpture, highly important Kashmir figure of Raktalokesvara, good 18th century Tibetan tanka of a Mahāsiddha, a fine pair of screens attribted to Kano Tanyu, highly important Nara dry lacquer figure of Monju</t>
-  </si>
-  <si>
-    <t>19770614, 19770615</t>
-  </si>
-  <si>
-    <t>approximately 72 pages</t>
-  </si>
-  <si>
-    <t>19771001</t>
-  </si>
-  <si>
-    <t>Japanese and other Asian works of art and a highly important American collection of early Japanese Buddhist &amp; Shinto paintings and sculptures (Part 1)</t>
-  </si>
-  <si>
-    <t>approximately 212 pages</t>
-  </si>
-  <si>
-    <t>a monumental Heian wood figure of a bodhisattva; a series of Chola and other Indian bronzes and stone; an early  Nepalese bronze of Syamatara; a fine Javanese bronze of Prajñāpāramitā; Japanese printings, sculpture, bronzes, lacquer, swords, fittings, prints, drawings, screens, ceramics, netsuke, inro, lacquer; Korean, Tibetan, Nepaliese, Indian and Southeast Asian works of art</t>
-  </si>
-  <si>
-    <t>19771103, 19771104</t>
-  </si>
-  <si>
-    <t>The contents of Mountain Crest, the collection of Mrs. Loyce Mayfield</t>
-  </si>
-  <si>
-    <t>approximately 96 pages</t>
-  </si>
-  <si>
-    <t>a fine collection of birds modelled by Dorothy Doughty and Edward Marshall Boehm, oriental works of arts, fine oriental rugs and carpets, Paul Storr George III silver soup tureen and cover, furniture and other decorative arts</t>
-  </si>
-  <si>
-    <t>19770610, 10770611</t>
-  </si>
-  <si>
-    <t>Chinese ceramics and works of art</t>
-  </si>
-  <si>
-    <t>approximately 116 pages</t>
-  </si>
-  <si>
-    <t>19771105</t>
-  </si>
-  <si>
-    <t>Chinese snuff bottles, jades, paintings, textiles and other works of art</t>
-  </si>
-  <si>
-    <t>[1978?]</t>
-  </si>
-  <si>
-    <t>© 1978</t>
-  </si>
-  <si>
-    <t>approximately 106 pages</t>
-  </si>
-  <si>
-    <t>19780125, 19780126</t>
-  </si>
-  <si>
-    <t>approximately 32 pages</t>
-  </si>
-  <si>
-    <t>19780304</t>
-  </si>
-  <si>
-    <t>19780128</t>
-  </si>
-  <si>
-    <t>Fine oriental miniatures, manuscripts, Islamic works of art, and 19th century paintings</t>
-  </si>
-  <si>
-    <t>[1979?]</t>
-  </si>
-  <si>
-    <t>© 1979</t>
-  </si>
-  <si>
-    <t>approximately 126 pages</t>
-  </si>
-  <si>
-    <t>19791214</t>
-  </si>
-  <si>
-    <t>Fine oriental miniatures, manuscripts, Islamic works of art, including the Fraser album</t>
-  </si>
-  <si>
-    <t>[1980?]</t>
-  </si>
-  <si>
-    <t>© 1980</t>
-  </si>
-  <si>
-    <t>approximately 136 pages</t>
-  </si>
-  <si>
-    <t>[property of various owners] including: property of Mr. Malcolm Fraser, property from the Estate of Nelson A. Rockefeller, property from the Estate of Mrs Benjamin Sonnenberg, property from the Hagop Kevorkian Fund</t>
-  </si>
-  <si>
-    <t>4493Y</t>
-  </si>
-  <si>
-    <t>19801209</t>
-  </si>
-  <si>
-    <t>Fine oriental miniatures, manuscripts, Islamic works of art</t>
-  </si>
-  <si>
-    <t>[1981?]</t>
-  </si>
-  <si>
-    <t>© 1981</t>
-  </si>
-  <si>
-    <t>approximately 120 pages</t>
-  </si>
-  <si>
-    <t>[property of various owners] including: the property of Mrs. Henry R. Gutnayer, New York; the property of Mr. and Mrs. Eugene Bernat; the property of Mr. Jack Josephson; the property of a New York collector; the property from the estate of Evelyn C. Byng</t>
-  </si>
-  <si>
-    <t>4618Y</t>
-  </si>
-  <si>
-    <t>19810521</t>
-  </si>
-  <si>
-    <t>[property of various owners] including: the property of Mr. T.B. Kahle, the property from the estate of Laila Y. Mathers, the property of Dr. and Mrs. Warren Baker, the property from the collection of the late Mr. Carleton Richmond</t>
-  </si>
-  <si>
-    <t>4756Y</t>
-  </si>
-  <si>
-    <t>19811210</t>
-  </si>
-  <si>
-    <t>Fine oriental miniatures, manuscripts and Islamic works of art</t>
-  </si>
-  <si>
-    <t>[1982?]</t>
-  </si>
-  <si>
-    <t>© 1982</t>
-  </si>
-  <si>
-    <t>approximately 104 pages</t>
-  </si>
-  <si>
-    <t>4867Y</t>
-  </si>
-  <si>
-    <t>19820519</t>
-  </si>
-  <si>
-    <t>Chinese and Japanese paintings, works of art and furniture</t>
-  </si>
-  <si>
-    <t>[1983?]</t>
-  </si>
-  <si>
-    <t>© 1983</t>
-  </si>
-  <si>
-    <t>approximately 100 pages</t>
-  </si>
-  <si>
-    <t>property of various owners including: property of the Newark Museum, property of the estate of Sophie H. Gimbel, property of the estate of Charlotte V. Bergen, Bernardsville, New Jersey. Sold by the order of the Trustees, Fidelity Union Bank, Newark, New Jersey. Property of Yves Saint Laurent, Inc. Property of the Albany Institute of History and Art. Property from the collection of the Late  Dr. and Mrs. Louis E. Wolferz, sold by order of the Heirs. Property of the estate of R. Foster Reynolds, Providence, Rhode Island. Property from the collection of Captain S. N. Ferris Luboshez USN (Ret'd). Property from the estate of Anne Burnett Tandy, Fort Worth, Texas.</t>
-  </si>
-  <si>
-    <t>19830226</t>
-  </si>
-  <si>
-    <t>Fine Japanese works of art including lacquer, ceramics, metalwork, enamels and paintings</t>
-  </si>
-  <si>
-    <t>[1984?]</t>
-  </si>
-  <si>
-    <t>© 1984</t>
-  </si>
-  <si>
-    <t>approximately 124 pages</t>
-  </si>
-  <si>
-    <t>19840331</t>
-  </si>
-  <si>
-    <t>Fine Oriental rugs and carpets</t>
-  </si>
-  <si>
-    <t>approximately 132 pages</t>
-  </si>
-  <si>
-    <t>property of various owners including: The Austin Family , Rosemont, Pennsylvania; The estate of Vladimir M. Eitingon; The estate of Reverend Joseph Madigan; The Ten Eyck Family, New York State; A London publishing house; A European gentleman</t>
-  </si>
-  <si>
-    <t>19840519</t>
-  </si>
-  <si>
-    <t>Fine Japanese prints, paintings, screens and decorative works of art</t>
-  </si>
-  <si>
-    <t>Including property from the Fichter collection of landscape prints and from the collection of Charles Hovey Pepper</t>
-  </si>
-  <si>
-    <t>27cm</t>
-  </si>
-  <si>
-    <t>SHAKUDO 5234</t>
-  </si>
-  <si>
-    <t>19841109, 19841110</t>
-  </si>
-  <si>
-    <t>The Salvatore J. Tarantino collection of woodblock prints by Ando Hiroshige (1797-1858) and fine woodblock prints, paintings and screens from various owners</t>
-  </si>
-  <si>
-    <t>Sotheby's Inc</t>
-  </si>
-  <si>
-    <t>[1985?]</t>
-  </si>
-  <si>
-    <t>© 1985</t>
-  </si>
-  <si>
-    <t>approximately 140 pages</t>
-  </si>
-  <si>
-    <t>TARANTINO 5385</t>
-  </si>
-  <si>
-    <t>19851106, 19851107</t>
-  </si>
-  <si>
-    <t>Fine Chinese snuff bottles</t>
-  </si>
-  <si>
-    <t>from the collection of Dr. Paula Hallett, immediately followed by snuff bottles the property of various owners</t>
-  </si>
-  <si>
-    <t>approximately 64 pages</t>
-  </si>
-  <si>
-    <t>MATRIX 5416</t>
-  </si>
-  <si>
-    <t>19851202</t>
-  </si>
-  <si>
-    <t>Fine Japanese prints, paintings, screens and works of art</t>
-  </si>
-  <si>
-    <t>[1986?]</t>
-  </si>
-  <si>
-    <t>© 1986</t>
-  </si>
-  <si>
-    <t>approximately  pages</t>
-  </si>
-  <si>
-    <t>YABU 5488</t>
-  </si>
-  <si>
-    <t>19860924</t>
-  </si>
-  <si>
-    <t>Fine Chinese paintings</t>
-  </si>
-  <si>
-    <t>Property of various owners, including the Kimbell Art Foundation, Fort Worth, Texas; Andrew Franklin, C.V.O. C.B.E., former British China  Consular Service; a European collection</t>
-  </si>
-  <si>
-    <t>[1987?]</t>
-  </si>
-  <si>
-    <t>© 1987</t>
-  </si>
-  <si>
-    <t>SONG KE 5591</t>
-  </si>
-  <si>
-    <t>19870602</t>
-  </si>
-  <si>
-    <t>Southeby's Arcade Auctions</t>
-  </si>
-  <si>
-    <t>Oriental and European rugs and carpets</t>
-  </si>
-  <si>
-    <t>approximately 44 pages</t>
-  </si>
-  <si>
-    <t>property of various owners including: property of the Metropolitan Museum of Art; property from the estate of Milford S. Worth; property of an Eastern private collector; property of a private collector, Pennsylvania</t>
-  </si>
-  <si>
-    <t>19870916</t>
-  </si>
-  <si>
-    <t>[1988?]</t>
-  </si>
-  <si>
-    <t>© 1988</t>
-  </si>
-  <si>
-    <t>approximately 36 pages</t>
-  </si>
-  <si>
-    <t>19880322</t>
-  </si>
-  <si>
-    <t>approximately 42 pages</t>
-  </si>
-  <si>
-    <t>property of various owners, including: the estate of George Kirkland Bishop; property from the estate of Caroline Ryan Foulke; property from the Estate of Sylvia Montag  Ferst; property of the Pacific Asia Museum, Pasadena, California; property from the estate of Belle Linsky, sold by the executors, Muriel Karasik and William D. Zabel; property from the Estate of Mrs. George Devendorf</t>
-  </si>
-  <si>
-    <t>19880928</t>
-  </si>
-  <si>
-    <t>Fine netsuke, inro and lacquer from the estate of Madelyn Hickmott</t>
-  </si>
-  <si>
-    <t>Sold for the benefit of the Hartford Foundation for Public Giving</t>
-  </si>
-  <si>
-    <t>[1989?]</t>
-  </si>
-  <si>
-    <t>© 1989</t>
-  </si>
-  <si>
-    <t>approximately 118 pages</t>
-  </si>
-  <si>
-    <t>HICKMOTT 5811</t>
-  </si>
-  <si>
-    <t>19890208</t>
-  </si>
-  <si>
-    <t>Fine Chinese decorative works of art</t>
-  </si>
-  <si>
-    <t>approximately 218 pages</t>
-  </si>
-  <si>
-    <t>property of various owners including: property of the Traphagen School Museum, New York; property from the estate of Madelyn Hickmott; property from the estate of William R. Lipscomb; property from a Miami Beach estate; property from a Northwest institution; property from the estate of Mr. and Mrs. Oliver Smalley; property from the collection of Philip Swingle</t>
-  </si>
-  <si>
-    <t>MEIXIAN 5897</t>
-  </si>
-  <si>
-    <t>19890928, 19890929</t>
-  </si>
-  <si>
-    <t>[1990?]</t>
-  </si>
-  <si>
-    <t>© 1990</t>
-  </si>
-  <si>
-    <t>approximately 230 pages</t>
-  </si>
-  <si>
-    <t>including: property from the estate of Frances C. Albee; property from the collection of Mrs. Elva Bernat; property from the collection of Mr. and Mrs. Jacques Brazy; property from the collection of John T. Dorrance, Jr.; property of a Florida collector; property from the collection of Maitland Lee Griggs; property from the estate of Madelyn Hickmott; property from the collection of Stanley J. Love; property from a Miami Beach estate; property from a private New Jersey collection; property from the estate of Mr. and Mrs. Oliver Smalley; property from the Smith-Walker Foundation; property from the collection of Ira H. Van Cleave; property from the collection of Frederick J. and Antoinette H. Van Syke</t>
-  </si>
-  <si>
-    <t>TINGQUA 5996</t>
-  </si>
-  <si>
-    <t>19900411, 19900412</t>
-  </si>
-  <si>
-    <t>approximately 174 pages</t>
-  </si>
-  <si>
-    <t>including property From the collection of the late Victoria Contag, formerly on loan to the Nelson-Atkins Museum. Kansas City, Missouri; Property From a European collection; property from an important private collection; property of the Sixuezhai collection</t>
-  </si>
-  <si>
-    <t>QICHANG 6027</t>
-  </si>
-  <si>
-    <t>19900530</t>
-  </si>
-  <si>
-    <t>approximately 210 pages</t>
-  </si>
-  <si>
-    <t>including property from the collection of the late Victoria Contag; property from the collection of John T. Dorrance; property from the collection of Dr. Robert J. Fanning; property from the estate of Richard B. Gump; property from a private Midwest collection; property of Mrs. Rafi Y. Mottahedeh; property of Sotheby's; property from the estate of Anoinette H. Van Slyke; property from the estate of Gordon Bailey Washburn</t>
-  </si>
-  <si>
-    <t>TAINAN 6074</t>
-  </si>
-  <si>
-    <t>19901018, 19901019</t>
-  </si>
-  <si>
-    <t>The Carter Burden collection of Indian paintings</t>
-  </si>
-  <si>
-    <t>[1991?]</t>
-  </si>
-  <si>
-    <t>© 1991</t>
-  </si>
-  <si>
-    <t>approximately 80 pages</t>
-  </si>
-  <si>
-    <t>PAHARI 6122</t>
-  </si>
-  <si>
-    <t>19910327</t>
-  </si>
-  <si>
-    <t>Indian and Southeast Asian art</t>
-  </si>
-  <si>
-    <t>including property of William H. Wolff, Inc.; property of Richard B. Gump, San Francisco; property from the collection of Carter Burden; property sold by the Los Angeles County Museum of Art to benefit future acquisitions; property of Dr. Kaywin Lehman Smith; property of the Ernest Erickson Foundation; works of art from the collection of the late Edgar J. Kaufman, Jr.</t>
-  </si>
-  <si>
-    <t>WOLFF 6146</t>
-  </si>
-  <si>
-    <t>Egyptian, Greek, Etruscan, Roman and Western Asiatic antiquities and Islamic works of art</t>
-  </si>
-  <si>
-    <t>including: a Roman bronze center table; an Attic marble grave stele, circa 360 B.C.; an Egyptian Chephren diorite jar, dynasty I-II; an Attic red-figure cup attributed to the school of Makron; a Roman marble head of Apollo; a Syrian limestone head of a god or prince; an Egyptian bronze mongoose; an Apulian red-figure pelike attibuted to the Lycurgus painter; a Cycladic marble pyxis, early bronze age II; a Roman marble cinerary vase, Flavian period; an Egyptian limestone relief of Akhenaten and Meritaten; a Roman bronze figure of Jupiter; an Egyptian limestone relief of the god Tutu; a Roman marble figure of Polyhymia</t>
-  </si>
-  <si>
-    <t>SENWOSRET 6196</t>
-  </si>
-  <si>
-    <t>19910618</t>
-  </si>
-  <si>
-    <t>[1992?]</t>
-  </si>
-  <si>
-    <t>© 1992</t>
-  </si>
-  <si>
-    <t>approximately 180 pages</t>
-  </si>
-  <si>
-    <t>XUANZAI 6306</t>
-  </si>
-  <si>
-    <t>19920601</t>
-  </si>
-  <si>
-    <t>Fine Chinese ceramics and works of art</t>
-  </si>
-  <si>
-    <t>including property from the collection of Maude Bouvier-Davis; property from the collection of Marlene Casey; property from a California estate; property from a Canadian collector; property from a Connecticut private collection; property from the collection of Sidney Day; property from an East Coast private collection; property from the estate of Helen Griiser; property of a Hong Kong private collection; property from the estate of William E. Little; property from the estate of Paul Martini, formerly in the collection of William Goadby Loew; property of a Maryland estate; property formerly in the estate of John Alex McCone, sold for the benefit of the McCone Foundation; property from the estate of Isabelle M. Murphy; property of a private New Jersey collection; property from a private collection; property from the collection of Adele Simpson; property of a southern museum; property from the estate of Thomas van Deusen; property from a Virginia private collection; property from the estate of S. Fulleron Weaver, East Hampton, New York; property from the estate of Ruth Weiss; property from the estate of William H. Wolff</t>
-  </si>
-  <si>
-    <t>QUEMOY 6308</t>
-  </si>
-  <si>
-    <t>19920603</t>
-  </si>
-  <si>
-    <t>Decorative works of art</t>
-  </si>
-  <si>
-    <t>Chinese, Japanese and Korean</t>
-  </si>
-  <si>
-    <t>approximately 190 pages</t>
-  </si>
-  <si>
-    <t>MONKEY 6312</t>
-  </si>
-  <si>
-    <t>19920606</t>
-  </si>
-  <si>
-    <t>[2001?]</t>
-  </si>
-  <si>
-    <t>152 pages</t>
-  </si>
-  <si>
-    <t>ELY 7622</t>
-  </si>
-  <si>
-    <t>20010322</t>
-  </si>
-  <si>
-    <t>236 pages</t>
-  </si>
-  <si>
-    <t>including important snuff bottles from a distinguished Asian collection</t>
-  </si>
-  <si>
-    <t>PRIMUS 7696</t>
-  </si>
-  <si>
-    <t>20010919</t>
-  </si>
-  <si>
-    <t>[2000?]</t>
-  </si>
-  <si>
-    <t>148 pages</t>
-  </si>
-  <si>
-    <t>ARUNDEL 7445</t>
-  </si>
-  <si>
-    <t>20000322</t>
-  </si>
-  <si>
-    <t>Important Chinese snuff bottles</t>
-  </si>
-  <si>
-    <t>[1997?]</t>
-  </si>
-  <si>
-    <t>© 1997</t>
-  </si>
-  <si>
-    <t>approximately 128 pages</t>
-  </si>
-  <si>
-    <t>including property from the John Franklin Dodge and Isabel Beatty Dodge Collection formed before 1965 (The Dodge Collection); property from The Pauline Lester Collection (Pauline Lester); property from a private Mid-Western American collection (The Mid-Western Collection); property from a private Canadian collection formed in Pekin before 1955 (The Canadian Collection); property from a private British Columbia Collection (The B.C. Collection); property from a private San Francisco collection (The S. F. Collection)</t>
-  </si>
-  <si>
-    <t>GOURD 6962</t>
-  </si>
-  <si>
-    <t>19970317</t>
-  </si>
-  <si>
-    <t>Fine Chinese Paintings</t>
-  </si>
-  <si>
-    <t>Asian Art</t>
-  </si>
-  <si>
-    <t>[1995?]</t>
-  </si>
-  <si>
-    <t>© 1995</t>
-  </si>
-  <si>
-    <t>approximately 160 pages</t>
-  </si>
-  <si>
-    <t>QIYUE 6738</t>
-  </si>
-  <si>
-    <t>19950918</t>
-  </si>
-  <si>
-    <t>[1993?]</t>
-  </si>
-  <si>
-    <t>© 1993</t>
-  </si>
-  <si>
-    <t>approximately 50 pages</t>
-  </si>
-  <si>
-    <t>including property of a private American collector</t>
-  </si>
-  <si>
-    <t>SHIPJANGSAENG 6441</t>
-  </si>
-  <si>
-    <t>19930618</t>
-  </si>
-  <si>
-    <t>Fine netsuke, inro and related works of art</t>
-  </si>
-  <si>
-    <t>Miami</t>
-  </si>
-  <si>
-    <t>MIAMI 5548</t>
-  </si>
-  <si>
-    <t>19870112</t>
-  </si>
-  <si>
-    <t>The Anne Paul Brinkman collection</t>
-  </si>
-  <si>
-    <t>ne</t>
-  </si>
-  <si>
-    <t>Amsterdam</t>
-  </si>
-  <si>
-    <t>Sotheby's Amsterdam B.V.</t>
-  </si>
-  <si>
-    <t>[2002?]</t>
-  </si>
-  <si>
-    <t>190 pages</t>
-  </si>
-  <si>
-    <t>AM0856</t>
-  </si>
-  <si>
-    <t>20020917</t>
-  </si>
-  <si>
-    <t>Rugs and carpets</t>
-  </si>
-  <si>
-    <t>From the collection of the late Mr. P. Otten, Amsterdam.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tapijten </t>
-  </si>
-  <si>
-    <t>Uit de verzameling van wijlen de heer Mr. P. Otten te Amsterdam</t>
-  </si>
-  <si>
-    <t>Sotheby Mak Van Waay B.V.</t>
-  </si>
-  <si>
-    <t>12 pages</t>
-  </si>
-  <si>
-    <t>19870706</t>
-  </si>
-  <si>
-    <t>Collection d'un amateur</t>
-  </si>
-  <si>
-    <t>Rouen 1680-1740: de la première porcelaine à l'âge d'or de la faïence</t>
-  </si>
-  <si>
-    <t>fr</t>
-  </si>
-  <si>
-    <t>Paris</t>
-  </si>
-  <si>
-    <t>Sotheby's France SA</t>
-  </si>
-  <si>
-    <t>[2008?]</t>
-  </si>
-  <si>
-    <t>166 pages</t>
-  </si>
-  <si>
-    <t>PF8025 ROUEN</t>
-  </si>
-  <si>
-    <t>20080618</t>
-  </si>
-  <si>
-    <t>Collection de monsieur et madame Luigi Anton Laura</t>
-  </si>
-  <si>
-    <t>Important mobilier, objets d'art et porcelaines de Chine</t>
-  </si>
-  <si>
-    <t>334 pages</t>
-  </si>
-  <si>
-    <t>28cm</t>
-  </si>
-  <si>
-    <t>PF1001 LAURA</t>
-  </si>
-  <si>
-    <t>20010627</t>
-  </si>
-  <si>
-    <t>Fine modern Chinese oil paintings, drawings and watercolours</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>Taipei</t>
-  </si>
-  <si>
-    <t>Sotheby's Taiwan Ltd.</t>
-  </si>
-  <si>
-    <t>SANXIA</t>
-  </si>
-  <si>
-    <t>19930418</t>
-  </si>
-  <si>
-    <t>La collezione Colasanti-Moore, Piazza dell'Orologio, Roma</t>
-  </si>
-  <si>
-    <t>it</t>
-  </si>
-  <si>
-    <t>Milan</t>
-  </si>
-  <si>
-    <t>Sotheby's Italia</t>
-  </si>
-  <si>
-    <t>181 pages</t>
-  </si>
-  <si>
-    <t>MI166 FABIOLA</t>
-  </si>
-  <si>
-    <t>20000229</t>
-  </si>
-  <si>
     <t>Oriental carpets</t>
   </si>
   <si>
@@ -1483,12 +1495,18 @@
     <t>19771024, 19771025, 19771026, 19771027</t>
   </si>
   <si>
+    <t>English / Chinese</t>
+  </si>
+  <si>
     <t>Southeby's Hong Kong spring sales 2007</t>
   </si>
   <si>
     <t>Southeby's Hong Kong 春李拍賣</t>
   </si>
   <si>
+    <t>Southeby's Hong Kong chun ji pai mai</t>
+  </si>
+  <si>
     <t>Southeby's Hong Kong</t>
   </si>
   <si>
@@ -1510,6 +1528,9 @@
     <t>香港蘇富比2010秋李拍賣</t>
   </si>
   <si>
+    <t>Xianggang Sufubi 2010 qiu ji pai mai</t>
+  </si>
+  <si>
     <t>[2010?]</t>
   </si>
   <si>
@@ -1531,6 +1552,9 @@
     <t>香港蘇富比2013秋李拍賣</t>
   </si>
   <si>
+    <t>Xianggang Sufubi 2013 qiu ji pai mai</t>
+  </si>
+  <si>
     <t>40: 蘇富比亞洲四十年</t>
   </si>
   <si>
@@ -1544,6 +1568,9 @@
   </si>
   <si>
     <t>約翰·法蘭寇收藏之常玉作品</t>
+  </si>
+  <si>
+    <t>Yuehan, Falankou shou cang zhi chang yu zuo pin</t>
   </si>
   <si>
     <t>Taiwan</t>
@@ -1832,7 +1859,8 @@
     <col customWidth="1" min="5" max="5" width="9.29"/>
     <col customWidth="1" min="6" max="6" width="14.29"/>
     <col customWidth="1" min="7" max="7" width="10.29"/>
-    <col customWidth="1" min="8" max="9" width="8.29"/>
+    <col customWidth="1" min="8" max="8" width="25.43"/>
+    <col customWidth="1" min="9" max="9" width="8.29"/>
     <col customWidth="1" min="10" max="10" width="19.86"/>
     <col customWidth="1" min="11" max="11" width="7.86"/>
     <col customWidth="1" min="12" max="12" width="12.43"/>
@@ -1935,7 +1963,7 @@
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1985,7 +2013,7 @@
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -2032,7 +2060,7 @@
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -2082,7 +2110,7 @@
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -2129,7 +2157,7 @@
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -2176,7 +2204,7 @@
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -2223,7 +2251,7 @@
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -2270,7 +2298,7 @@
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -2317,7 +2345,7 @@
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -2361,7 +2389,7 @@
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -2408,7 +2436,7 @@
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -2455,7 +2483,7 @@
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -2502,7 +2530,7 @@
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -2552,7 +2580,7 @@
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -2602,7 +2630,7 @@
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -2652,7 +2680,7 @@
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -2699,7 +2727,7 @@
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -2746,7 +2774,7 @@
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -2790,7 +2818,7 @@
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -2837,7 +2865,7 @@
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="2"/>
@@ -2885,7 +2913,7 @@
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C22" s="2"/>
@@ -2930,7 +2958,7 @@
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="2"/>
@@ -2978,7 +3006,7 @@
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="2"/>
@@ -3023,7 +3051,7 @@
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="2"/>
@@ -3071,7 +3099,7 @@
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="2"/>
@@ -3122,7 +3150,7 @@
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="2"/>
@@ -3173,7 +3201,7 @@
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="2"/>
@@ -3224,7 +3252,7 @@
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="2"/>
@@ -3272,7 +3300,7 @@
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C30" s="2"/>
@@ -3320,7 +3348,7 @@
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="2"/>
@@ -3368,7 +3396,7 @@
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="2"/>
@@ -3416,7 +3444,7 @@
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C33" s="2"/>
@@ -3464,7 +3492,7 @@
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C34" s="2"/>
@@ -3509,7 +3537,7 @@
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C35" s="2"/>
@@ -3557,7 +3585,7 @@
       <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C36" s="2"/>
@@ -3605,7 +3633,7 @@
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C37" s="2"/>
@@ -3653,7 +3681,7 @@
       <c r="A38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C38" s="2"/>
@@ -3701,7 +3729,7 @@
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C39" s="2"/>
@@ -3749,7 +3777,7 @@
       <c r="A40" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C40" s="2"/>
@@ -3791,7 +3819,7 @@
       <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C41" s="2"/>
@@ -3836,7 +3864,7 @@
       <c r="A42" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C42" s="2"/>
@@ -3878,7 +3906,7 @@
       <c r="A43" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C43" s="2"/>
@@ -3926,7 +3954,7 @@
       <c r="A44" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C44" s="2"/>
@@ -3974,7 +4002,7 @@
       <c r="A45" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C45" s="2"/>
@@ -4025,7 +4053,7 @@
       <c r="A46" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C46" s="2"/>
@@ -4070,7 +4098,7 @@
       <c r="A47" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C47" s="2"/>
@@ -4113,21 +4141,21 @@
       <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>27</v>
+      <c r="B48" s="3" t="s">
+        <v>254</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>247</v>
@@ -4136,7 +4164,7 @@
         <v>248</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="O48" s="2" t="s">
         <v>141</v>
@@ -4145,7 +4173,7 @@
         <v>142</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="R48" s="1" t="s">
         <v>118</v>
@@ -4154,7 +4182,7 @@
         <v>461.0</v>
       </c>
       <c r="W48" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="Y48" s="3" t="s">
         <v>39</v>
@@ -4167,40 +4195,40 @@
       <c r="A49" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>27</v>
+      <c r="B49" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="P49" s="2"/>
       <c r="Q49" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="R49" s="1" t="s">
         <v>118</v>
       </c>
       <c r="V49" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="W49" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="Y49" s="3" t="s">
         <v>39</v>
@@ -4213,40 +4241,40 @@
       <c r="A50" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>27</v>
+      <c r="B50" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="O50" s="2" t="s">
         <v>210</v>
       </c>
       <c r="P50" s="2"/>
       <c r="Q50" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="R50" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="V50" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="W50" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="Y50" s="3" t="s">
         <v>39</v>
@@ -4259,21 +4287,21 @@
       <c r="A51" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>27</v>
+      <c r="B51" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="O51" s="2" t="s">
         <v>236</v>
@@ -4286,10 +4314,10 @@
         <v>118</v>
       </c>
       <c r="V51" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="W51" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="Y51" s="3" t="s">
         <v>39</v>
@@ -4302,37 +4330,37 @@
       <c r="A52" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>27</v>
+      <c r="B52" s="3" t="s">
+        <v>284</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="O52" s="2" t="s">
         <v>218</v>
       </c>
       <c r="P52" s="2"/>
       <c r="Q52" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="R52" s="1" t="s">
         <v>118</v>
       </c>
       <c r="V52" s="1" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="W52" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="Y52" s="3" t="s">
         <v>39</v>
@@ -4346,20 +4374,20 @@
         <v>26</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="O53" s="2" t="s">
         <v>123</v>
@@ -4374,10 +4402,10 @@
         <v>118</v>
       </c>
       <c r="V53" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="W53" s="2" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="Y53" s="3" t="s">
         <v>39</v>
@@ -4391,20 +4419,20 @@
         <v>26</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="O54" s="2" t="s">
         <v>108</v>
@@ -4413,16 +4441,16 @@
         <v>124</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="R54" s="1" t="s">
         <v>118</v>
       </c>
       <c r="V54" s="1" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="W54" s="2" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="Y54" s="3" t="s">
         <v>39</v>
@@ -4436,20 +4464,20 @@
         <v>26</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="1" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="O55" s="2" t="s">
         <v>123</v>
@@ -4458,16 +4486,16 @@
         <v>124</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="R55" s="1" t="s">
         <v>118</v>
       </c>
       <c r="V55" s="1" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="W55" s="2" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="Y55" s="3" t="s">
         <v>39</v>
@@ -4481,20 +4509,20 @@
         <v>26</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="N56" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="N56" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="O56" s="2" t="s">
         <v>123</v>
@@ -4503,16 +4531,16 @@
         <v>124</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="R56" s="1" t="s">
         <v>118</v>
       </c>
       <c r="V56" s="1" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="W56" s="2" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="Y56" s="3" t="s">
         <v>39</v>
@@ -4526,20 +4554,20 @@
         <v>26</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="1" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="O57" s="2" t="s">
         <v>141</v>
@@ -4548,16 +4576,16 @@
         <v>142</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="R57" s="1" t="s">
         <v>118</v>
       </c>
       <c r="V57" s="1" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="W57" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="Y57" s="3" t="s">
         <v>39</v>
@@ -4571,20 +4599,20 @@
         <v>26</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="1" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="O58" s="2" t="s">
         <v>159</v>
@@ -4593,19 +4621,19 @@
         <v>160</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="R58" s="1" t="s">
         <v>118</v>
       </c>
       <c r="U58" s="1" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="V58" s="1" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="W58" s="2" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="Y58" s="3" t="s">
         <v>39</v>
@@ -4619,20 +4647,20 @@
         <v>26</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="1" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="O59" s="2" t="s">
         <v>184</v>
@@ -4647,13 +4675,13 @@
         <v>118</v>
       </c>
       <c r="U59" s="1" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="V59" s="1" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="W59" s="2" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="Y59" s="3" t="s">
         <v>39</v>
@@ -4667,20 +4695,20 @@
         <v>26</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="1" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="O60" s="2" t="s">
         <v>196</v>
@@ -4689,19 +4717,19 @@
         <v>197</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="R60" s="1" t="s">
         <v>118</v>
       </c>
       <c r="U60" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="V60" s="1" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="W60" s="2" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="Y60" s="3" t="s">
         <v>39</v>
@@ -4715,20 +4743,20 @@
         <v>26</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="1" t="s">
         <v>128</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="O61" s="2" t="s">
         <v>196</v>
@@ -4743,13 +4771,13 @@
         <v>118</v>
       </c>
       <c r="U61" s="1" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="V61" s="1" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="W61" s="2" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="Y61" s="3" t="s">
         <v>39</v>
@@ -4763,20 +4791,20 @@
         <v>26</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="O62" s="2" t="s">
         <v>236</v>
@@ -4791,10 +4819,10 @@
         <v>118</v>
       </c>
       <c r="V62" s="1" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="W62" s="2" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="Y62" s="3" t="s">
         <v>39</v>
@@ -4808,41 +4836,41 @@
         <v>26</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="1" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="P63" s="2" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="Q63" s="1" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="R63" s="1" t="s">
         <v>118</v>
       </c>
       <c r="U63" s="1" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="V63" s="1" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="W63" s="2" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="Y63" s="3" t="s">
         <v>39</v>
@@ -4856,41 +4884,41 @@
         <v>26</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="1" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="O64" s="2" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="P64" s="2" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="Q64" s="1" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="R64" s="1" t="s">
         <v>118</v>
       </c>
       <c r="U64" s="1" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="V64" s="1" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="W64" s="2" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="Y64" s="3" t="s">
         <v>39</v>
@@ -4904,36 +4932,36 @@
         <v>26</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="1" t="s">
         <v>201</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="O65" s="2" t="s">
         <v>218</v>
       </c>
       <c r="P65" s="2"/>
       <c r="Q65" s="1" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="R65" s="1" t="s">
         <v>118</v>
       </c>
       <c r="V65" s="1" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="W65" s="2" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="Y65" s="3" t="s">
         <v>39</v>
@@ -4947,36 +4975,36 @@
         <v>26</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="1" t="s">
         <v>201</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="O66" s="2" t="s">
         <v>210</v>
       </c>
       <c r="P66" s="2"/>
       <c r="Q66" s="1" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="R66" s="1" t="s">
         <v>118</v>
       </c>
       <c r="V66" s="1" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="W66" s="2" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="Y66" s="3" t="s">
         <v>39</v>
@@ -4990,39 +5018,39 @@
         <v>26</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="1" t="s">
         <v>201</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="O67" s="2" t="s">
         <v>250</v>
       </c>
       <c r="P67" s="2"/>
       <c r="Q67" s="1" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="R67" s="1" t="s">
         <v>118</v>
       </c>
       <c r="V67" s="1" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="W67" s="2" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="Y67" s="3" t="s">
         <v>39</v>
@@ -5036,36 +5064,36 @@
         <v>26</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="1" t="s">
         <v>201</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="O68" s="2" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="P68" s="2"/>
       <c r="Q68" s="1" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="R68" s="1" t="s">
         <v>118</v>
       </c>
       <c r="V68" s="1" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="W68" s="2" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="Y68" s="3" t="s">
         <v>39</v>
@@ -5079,39 +5107,39 @@
         <v>26</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="1" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="O69" s="2" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="P69" s="2"/>
       <c r="Q69" s="1" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="R69" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="V69" s="1" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="W69" s="2" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="Y69" s="3" t="s">
         <v>39</v>
@@ -5125,42 +5153,42 @@
         <v>26</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="1" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="P70" s="2"/>
       <c r="Q70" s="1" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="R70" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="U70" s="1" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="V70" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="W70" s="2" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="Y70" s="3" t="s">
         <v>39</v>
@@ -5174,42 +5202,42 @@
         <v>26</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="1" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="O71" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="P71" s="2"/>
       <c r="Q71" s="1" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="R71" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="U71" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="V71" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="W71" s="2" t="s">
         <v>371</v>
-      </c>
-      <c r="U71" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="V71" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="W71" s="2" t="s">
-        <v>367</v>
       </c>
       <c r="Y71" s="3" t="s">
         <v>39</v>
@@ -5223,42 +5251,42 @@
         <v>26</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="1" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="O72" s="2" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="P72" s="2"/>
       <c r="Q72" s="1" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="R72" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="U72" s="1" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="V72" s="1" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="W72" s="2" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="Y72" s="3" t="s">
         <v>39</v>
@@ -5272,39 +5300,39 @@
         <v>26</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="1" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="O73" s="2" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="P73" s="2"/>
       <c r="Q73" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="R73" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="U73" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="R73" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="U73" s="1" t="s">
-        <v>378</v>
-      </c>
       <c r="V73" s="1" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="W73" s="2" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="Y73" s="3" t="s">
         <v>39</v>
@@ -5318,39 +5346,39 @@
         <v>26</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="1" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="O74" s="2" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="P74" s="2"/>
       <c r="Q74" s="1" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="R74" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="U74" s="1" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="V74" s="1" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="W74" s="2" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="Y74" s="3" t="s">
         <v>39</v>
@@ -5364,38 +5392,38 @@
         <v>26</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="1" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="O75" s="2" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="P75" s="2" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="Q75" s="1" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="R75" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U75" s="1" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="W75" s="2" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="Y75" s="3" t="s">
         <v>39</v>
@@ -5409,38 +5437,38 @@
         <v>26</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="1" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="P76" s="2" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="Q76" s="1" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="R76" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U76" s="1" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="W76" s="2" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="Y76" s="3" t="s">
         <v>39</v>
@@ -5454,20 +5482,20 @@
         <v>26</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="1" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="O77" s="2" t="s">
         <v>32</v>
@@ -5476,16 +5504,16 @@
         <v>33</v>
       </c>
       <c r="Q77" s="1" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="R77" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U77" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="W77" s="2" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="Y77" s="3" t="s">
         <v>39</v>
@@ -5499,20 +5527,20 @@
         <v>26</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="1" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="O78" s="2" t="s">
         <v>32</v>
@@ -5521,19 +5549,19 @@
         <v>33</v>
       </c>
       <c r="Q78" s="1" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="R78" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U78" s="1" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="V78" s="1" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="W78" s="2" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="Y78" s="3" t="s">
         <v>39</v>
@@ -5547,20 +5575,20 @@
         <v>26</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="1" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="O79" s="2" t="s">
         <v>32</v>
@@ -5569,19 +5597,19 @@
         <v>33</v>
       </c>
       <c r="Q79" s="1" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="R79" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U79" s="1" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="V79" s="1" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="W79" s="2" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="Y79" s="3" t="s">
         <v>39</v>
@@ -5595,20 +5623,20 @@
         <v>26</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="1" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="O80" s="2" t="s">
         <v>32</v>
@@ -5617,19 +5645,19 @@
         <v>33</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="R80" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U80" s="1" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="V80" s="1" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="W80" s="2" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="Y80" s="3" t="s">
         <v>39</v>
@@ -5643,23 +5671,23 @@
         <v>26</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="1" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="O81" s="2" t="s">
         <v>74</v>
@@ -5671,16 +5699,16 @@
         <v>147</v>
       </c>
       <c r="R81" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U81" s="1" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="V81" s="1" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="W81" s="2" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="Y81" s="3" t="s">
         <v>39</v>
@@ -5694,20 +5722,20 @@
         <v>26</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="1" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="L82" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="O82" s="2" t="s">
         <v>74</v>
@@ -5716,19 +5744,19 @@
         <v>75</v>
       </c>
       <c r="Q82" s="1" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="R82" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U82" s="1" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="V82" s="1" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="W82" s="2" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="Y82" s="3" t="s">
         <v>39</v>
@@ -5742,20 +5770,20 @@
         <v>26</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="1" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="L83" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="O83" s="2" t="s">
         <v>79</v>
@@ -5764,16 +5792,16 @@
         <v>80</v>
       </c>
       <c r="Q83" s="1" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="R83" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="V83" s="1" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="W83" s="2" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="Y83" s="3" t="s">
         <v>39</v>
@@ -5787,20 +5815,20 @@
         <v>26</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="L84" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="N84" s="1" t="s">
         <v>432</v>
-      </c>
-      <c r="L84" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="M84" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="N84" s="1" t="s">
-        <v>428</v>
       </c>
       <c r="O84" s="2" t="s">
         <v>79</v>
@@ -5809,19 +5837,19 @@
         <v>80</v>
       </c>
       <c r="Q84" s="1" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="R84" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U84" s="1" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="V84" s="1" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="W84" s="2" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="Y84" s="3" t="s">
         <v>39</v>
@@ -5835,42 +5863,42 @@
         <v>26</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="1" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="L85" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="O85" s="2" t="s">
         <v>79</v>
       </c>
       <c r="P85" s="2"/>
       <c r="Q85" s="1" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="R85" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U85" s="1" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="V85" s="1" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="W85" s="2" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="Y85" s="3" t="s">
         <v>39</v>
@@ -5884,20 +5912,20 @@
         <v>26</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="1" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="O86" s="2" t="s">
         <v>86</v>
@@ -5907,13 +5935,13 @@
         <v>130</v>
       </c>
       <c r="R86" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="V86" s="1" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="W86" s="2" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="Y86" s="3" t="s">
         <v>39</v>
@@ -5927,20 +5955,20 @@
         <v>26</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="1" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="O87" s="2" t="s">
         <v>86</v>
@@ -5950,13 +5978,13 @@
         <v>130</v>
       </c>
       <c r="R87" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="V87" s="1" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="W87" s="2" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="Y87" s="3" t="s">
         <v>39</v>
@@ -5970,20 +5998,20 @@
         <v>26</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="O88" s="2" t="s">
         <v>86</v>
@@ -5992,19 +6020,19 @@
         <v>87</v>
       </c>
       <c r="Q88" s="1" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="R88" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U88" s="1" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="V88" s="1" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="W88" s="2" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="Y88" s="3" t="s">
         <v>39</v>
@@ -6018,20 +6046,20 @@
         <v>26</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="1" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="O89" s="2" t="s">
         <v>86</v>
@@ -6040,19 +6068,19 @@
         <v>87</v>
       </c>
       <c r="Q89" s="1" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="R89" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U89" s="1" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="V89" s="1" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="W89" s="2" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="Y89" s="3" t="s">
         <v>39</v>
@@ -6066,20 +6094,20 @@
         <v>26</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="1" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="O90" s="2" t="s">
         <v>86</v>
@@ -6088,19 +6116,19 @@
         <v>87</v>
       </c>
       <c r="Q90" s="1" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="R90" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U90" s="1" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="V90" s="1" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="W90" s="2" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="Y90" s="3" t="s">
         <v>39</v>
@@ -6114,23 +6142,23 @@
         <v>26</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="1" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="O91" s="2" t="s">
         <v>74</v>
@@ -6139,19 +6167,19 @@
         <v>75</v>
       </c>
       <c r="Q91" s="1" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="R91" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U91" s="1" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="V91" s="1" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="W91" s="2" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="Y91" s="3" t="s">
         <v>39</v>
@@ -6165,23 +6193,23 @@
         <v>26</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="L92" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="N92" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="L92" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="M92" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="N92" s="1" t="s">
-        <v>462</v>
       </c>
       <c r="O92" s="2" t="s">
         <v>74</v>
@@ -6190,19 +6218,19 @@
         <v>75</v>
       </c>
       <c r="Q92" s="1" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="R92" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U92" s="1" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="V92" s="1" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="W92" s="2" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="Y92" s="3" t="s">
         <v>39</v>
@@ -6216,23 +6244,23 @@
         <v>26</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="1" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="M93" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="O93" s="2" t="s">
         <v>96</v>
@@ -6241,19 +6269,19 @@
         <v>97</v>
       </c>
       <c r="Q93" s="1" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="R93" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="U93" s="1" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="V93" s="1" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="W93" s="2" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="Y93" s="3" t="s">
         <v>39</v>
@@ -6267,23 +6295,23 @@
         <v>26</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="1" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="L94" s="1" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="M94" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="O94" s="2" t="s">
         <v>86</v>
@@ -6292,19 +6320,19 @@
         <v>87</v>
       </c>
       <c r="Q94" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="R94" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="U94" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="R94" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="U94" s="1" t="s">
-        <v>475</v>
-      </c>
       <c r="V94" s="1" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="W94" s="2" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="Y94" s="3" t="s">
         <v>39</v>
@@ -6318,20 +6346,20 @@
         <v>26</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="1" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="O95" s="2" t="s">
         <v>32</v>
@@ -6340,19 +6368,19 @@
         <v>33</v>
       </c>
       <c r="Q95" s="1" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="R95" s="1" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="U95" s="1" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="V95" s="1" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="W95" s="2" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="Y95" s="3" t="s">
         <v>39</v>
@@ -6365,40 +6393,43 @@
       <c r="A96" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>27</v>
+      <c r="B96" s="3" t="s">
+        <v>494</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="1" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>491</v>
+        <v>496</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>497</v>
       </c>
       <c r="L96" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="O96" s="2" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="P96" s="2"/>
       <c r="Q96" s="1" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="R96" s="1" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="U96" s="1" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="W96" s="2" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="Y96" s="3" t="s">
         <v>39</v>
@@ -6411,37 +6442,40 @@
       <c r="A97" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>27</v>
+      <c r="B97" s="3" t="s">
+        <v>494</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="1" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="H97" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="M97" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="N97" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="L97" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="M97" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="N97" s="1" t="s">
-        <v>492</v>
-      </c>
       <c r="O97" s="2" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="P97" s="2"/>
       <c r="Q97" s="1" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="R97" s="1" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="W97" s="2" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="Y97" s="3" t="s">
         <v>39</v>
@@ -6454,33 +6488,36 @@
       <c r="A98" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>27</v>
+      <c r="B98" s="3" t="s">
+        <v>494</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="1" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>505</v>
+        <v>512</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>513</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="L98" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="O98" s="2" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="P98" s="2"/>
       <c r="Q98" s="1" t="s">
@@ -6490,7 +6527,7 @@
         <v>118</v>
       </c>
       <c r="W98" s="2" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
       <c r="Y98" s="3" t="s">
         <v>39</v>
@@ -6503,40 +6540,43 @@
       <c r="A99" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>27</v>
+      <c r="B99" s="3" t="s">
+        <v>494</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="1" t="s">
-        <v>509</v>
+        <v>517</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>510</v>
+        <v>518</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>519</v>
       </c>
       <c r="L99" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M99" s="1" t="s">
-        <v>511</v>
+        <v>520</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>512</v>
+        <v>521</v>
       </c>
       <c r="O99" s="2" t="s">
         <v>231</v>
       </c>
       <c r="P99" s="2"/>
       <c r="Q99" s="1" t="s">
-        <v>513</v>
+        <v>522</v>
       </c>
       <c r="R99" s="1" t="s">
         <v>118</v>
       </c>
       <c r="V99" s="1" t="s">
-        <v>514</v>
+        <v>523</v>
       </c>
       <c r="W99" s="2" t="s">
-        <v>515</v>
+        <v>524</v>
       </c>
       <c r="Y99" s="3" t="s">
         <v>39</v>

</xml_diff>